<commit_message>
data : case 4
</commit_message>
<xml_diff>
--- a/data/case1/16/P1_4.xlsx
+++ b/data/case1/16/P1_4.xlsx
@@ -61,167 +61,167 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>0.23554697474668274</v>
+        <v>0.24002744690420741</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>-0.0099999972880553401</v>
+        <v>-0.0099999987598664575</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>-0.0089999972778134207</v>
+        <v>-0.0089999987555042793</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.061978859230237049</v>
+        <v>0.061988487830195282</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>-0.0059999973367323989</v>
+        <v>-0.005999998785518379</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>-0.0059999972894395626</v>
+        <v>-0.0059999987632366469</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>-0.019999996899331407</v>
+        <v>-0.01999999856293222</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>-0.01999999688620413</v>
+        <v>-0.019999998555569221</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>-0.0059999972615125685</v>
+        <v>-0.0059999987471863747</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>-0.0059999972557136516</v>
+        <v>-0.0059999987431496038</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>-0.0044999972968469137</v>
+        <v>-0.0044999987641816119</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>-0.0059999972556434855</v>
+        <v>-0.0059999987426446744</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.063252762479462099</v>
+        <v>0.054437725003959159</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>-0.011999997079272795</v>
+        <v>-0.01199999865125978</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>-0.023077344996194071</v>
+        <v>-0.019116548861301652</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>-0.0059999972229811682</v>
+        <v>-0.0059999987260574983</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>-0.0059999972132445123</v>
+        <v>-0.0059999987212204786</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>-0.0089999971297887171</v>
+        <v>-0.0089999986779991659</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>-0.0089999973152918855</v>
+        <v>-0.0089999987723698993</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>-0.0089999972367049708</v>
+        <v>-0.0089999987362290312</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>-0.0089999972210774715</v>
+        <v>-0.0089999987286750738</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>-0.061078720136420905</v>
+        <v>-0.062351734190375208</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>-0.0089999972555201424</v>
+        <v>-0.0089999987442466178</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>-0.041999996303732523</v>
+        <v>-0.041999998258022586</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>-0.041999996284213026</v>
+        <v>-0.041999998248549275</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>-0.0059999972887254671</v>
+        <v>-0.0059999987626753182</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>-0.0059999972875859342</v>
+        <v>-0.0059999987618954975</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>-0.0059999972791864309</v>
+        <v>-0.0059999987584768988</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>-0.011999997111448835</v>
+        <v>-0.01199999867276702</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>-0.019999996892094529</v>
+        <v>-0.019999998560271237</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.06147069836938357</v>
+        <v>0.062494406107528988</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>-0.031090958983376993</v>
+        <v>-0.030264408750954708</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>-0.0059999972847020189</v>
+        <v>-0.0059999987619150374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>